<commit_message>
changed the xls file
</commit_message>
<xml_diff>
--- a/Project-Links.xlsx
+++ b/Project-Links.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Bitbop DE</t>
   </si>
@@ -37,13 +37,31 @@
   </si>
   <si>
     <t>https://github.com/</t>
+  </si>
+  <si>
+    <t>http://www.stage-bitbop.com/admin</t>
+  </si>
+  <si>
+    <t>http://www.bitbop.com/admin</t>
+  </si>
+  <si>
+    <t>http://www.-bitbop.de/admin</t>
+  </si>
+  <si>
+    <t>http://www.stage-bitbop.de/admin</t>
+  </si>
+  <si>
+    <t>Staging admin</t>
+  </si>
+  <si>
+    <t>Production admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +76,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,19 +111,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,15 +422,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" thickBot="1">
@@ -407,7 +439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1">
+    <row r="2" spans="1:2" ht="15" thickTop="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -428,14 +460,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickTop="1"/>
-    <row r="8" spans="1:2" ht="18" thickBot="1">
-      <c r="A8" s="2" t="s">
+    <row r="6" spans="1:2" ht="15" thickTop="1">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" ht="18" thickBot="1">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickTop="1"/>
+    <row r="10" spans="1:2" ht="15" thickTop="1">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -446,7 +517,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -458,7 +529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>